<commit_message>
feat: Implement frontend API client and establish Playwright E2E testing framework with custom Excel reporting.
</commit_message>
<xml_diff>
--- a/frontend/tests/test-results/ShopEase_TestReport.xlsx
+++ b/frontend/tests/test-results/ShopEase_TestReport.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="215">
   <si>
     <t>ShopEase E2E Test Execution Report</t>
   </si>
@@ -21,13 +21,13 @@
     <t>Generated:</t>
   </si>
   <si>
-    <t>22/2/2026, 12:36:05 am</t>
+    <t>22/2/2026, 11:44:16 am</t>
   </si>
   <si>
     <t>Duration:</t>
   </si>
   <si>
-    <t>292s</t>
+    <t>434s</t>
   </si>
   <si>
     <t>Metric</t>
@@ -51,7 +51,7 @@
     <t>Pass Rate</t>
   </si>
   <si>
-    <t>50.0%</t>
+    <t>14.5%</t>
   </si>
   <si>
     <t>Module</t>
@@ -78,9 +78,33 @@
     <t>Error</t>
   </si>
   <si>
+    <t>ADMIN — Access</t>
+  </si>
+  <si>
+    <t>ADM-N01</t>
+  </si>
+  <si>
+    <t>Unauthenticated user cannot access /admin</t>
+  </si>
+  <si>
+    <t>Negative</t>
+  </si>
+  <si>
     <t>chromium</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t>ADM-N02</t>
+  </si>
+  <si>
+    <t>Customer role cannot access /admin</t>
+  </si>
+  <si>
+    <t>AUTH — Registration</t>
+  </si>
+  <si>
     <t>AUTH-P01</t>
   </si>
   <si>
@@ -90,16 +114,7 @@
     <t>Positive</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>ADM-N01</t>
-  </si>
-  <si>
-    <t>Unauthenticated user cannot access /admin</t>
-  </si>
-  <si>
-    <t>Negative</t>
+    <t>Error: [2mexpect([22m[31mpage[39m[2m).not.[22mtoHaveURL[2m([22m[32mexpected[39m[2m)[22m failed</t>
   </si>
   <si>
     <t>AUTH-N01</t>
@@ -114,10 +129,16 @@
     <t>Registration fails with short password</t>
   </si>
   <si>
-    <t>ADM-N02</t>
-  </si>
-  <si>
-    <t>Customer role cannot access /admin</t>
+    <t>ADM-P01</t>
+  </si>
+  <si>
+    <t>Admin user can access /admin dashboard</t>
+  </si>
+  <si>
+    <t>Error: [2mexpect([22m[31mlocator[39m[2m).[22mtoBeVisible[2m([22m[2m)[22m failed</t>
+  </si>
+  <si>
+    <t>AUTH — Login</t>
   </si>
   <si>
     <t>AUTH-P02</t>
@@ -126,16 +147,13 @@
     <t>Customer can login with valid credentials</t>
   </si>
   <si>
-    <t>Error: [2mexpect([22m[31mlocator[39m[2m).[22mtoContainText[2m([22m[32mexpected[39m[2m)[22m failed</t>
-  </si>
-  <si>
-    <t>ADM-P01</t>
-  </si>
-  <si>
-    <t>Admin user can access /admin dashboard</t>
-  </si>
-  <si>
-    <t>Error: [2mexpect([22m[31mlocator[39m[2m).[22mtoBeVisible[2m([22m[2m)[22m failed</t>
+    <t>ADMIN — Dashboard</t>
+  </si>
+  <si>
+    <t>ADM-P02</t>
+  </si>
+  <si>
+    <t>Dashboard shows stats: total users, total orders, total revenue</t>
   </si>
   <si>
     <t>AUTH-P03</t>
@@ -150,16 +168,22 @@
     <t>Login fails with wrong password</t>
   </si>
   <si>
+    <t>ADMIN — Orders</t>
+  </si>
+  <si>
+    <t>ADM-P03</t>
+  </si>
+  <si>
+    <t>Orders tab shows list of all orders</t>
+  </si>
+  <si>
     <t>AUTH-N04</t>
   </si>
   <si>
     <t>Login fails with non-existent email</t>
   </si>
   <si>
-    <t>ADM-P02</t>
-  </si>
-  <si>
-    <t>Dashboard shows stats: total users, total orders, total revenue</t>
+    <t>AUTH — Guard</t>
   </si>
   <si>
     <t>AUTH-N05</t>
@@ -168,6 +192,12 @@
     <t>Unauthenticated user is redirected from /profile</t>
   </si>
   <si>
+    <t>ADM-P04</t>
+  </si>
+  <si>
+    <t>Admin can update order status</t>
+  </si>
+  <si>
     <t>AUTH-N06</t>
   </si>
   <si>
@@ -180,19 +210,34 @@
     <t>Non-admin user cannot access /admin</t>
   </si>
   <si>
-    <t>ADM-P03</t>
-  </si>
-  <si>
-    <t>Orders tab shows list of all orders</t>
+    <t>ADMIN — Coupons</t>
+  </si>
+  <si>
+    <t>ADM-P05</t>
+  </si>
+  <si>
+    <t>Coupons tab shows list of all coupons</t>
+  </si>
+  <si>
+    <t>AUTH — Logout</t>
+  </si>
+  <si>
+    <t>AUTH-P04</t>
+  </si>
+  <si>
+    <t>User can logout</t>
   </si>
   <si>
     <t>TimeoutError: locator.click: Timeout 10000ms exceeded.</t>
   </si>
   <si>
-    <t>AUTH-P04</t>
-  </si>
-  <si>
-    <t>User can logout</t>
+    <t>ADM-P06</t>
+  </si>
+  <si>
+    <t>Admin can create a new coupon</t>
+  </si>
+  <si>
+    <t>CART — Add</t>
   </si>
   <si>
     <t>CART-P01</t>
@@ -201,10 +246,10 @@
     <t>Logged-in user can add a product to cart from product detail</t>
   </si>
   <si>
-    <t>ADM-P04</t>
-  </si>
-  <si>
-    <t>Admin can update order status</t>
+    <t>ADM-N03</t>
+  </si>
+  <si>
+    <t>Creating coupon with duplicate code shows error</t>
   </si>
   <si>
     <t>CART-P02</t>
@@ -213,10 +258,10 @@
     <t>Cart count updates in navbar after adding product</t>
   </si>
   <si>
-    <t>ADM-P05</t>
-  </si>
-  <si>
-    <t>Coupons tab shows list of all coupons</t>
+    <t>ADM-P07</t>
+  </si>
+  <si>
+    <t>Admin can delete a coupon</t>
   </si>
   <si>
     <t>CART-N01</t>
@@ -225,10 +270,16 @@
     <t>Unauthenticated user is prompted to login when adding to cart</t>
   </si>
   <si>
-    <t>ADM-P06</t>
-  </si>
-  <si>
-    <t>Admin can create a new coupon</t>
+    <t>ADMIN — Users</t>
+  </si>
+  <si>
+    <t>ADM-P08</t>
+  </si>
+  <si>
+    <t>Users tab shows list of registered users</t>
+  </si>
+  <si>
+    <t>CART — View</t>
   </si>
   <si>
     <t>CART-P03</t>
@@ -237,10 +288,10 @@
     <t>Cart page shows added items</t>
   </si>
   <si>
-    <t>ADM-N03</t>
-  </si>
-  <si>
-    <t>Creating coupon with duplicate code shows error</t>
+    <t>ADM-P09</t>
+  </si>
+  <si>
+    <t>Users list shows at least one user (seed data)</t>
   </si>
   <si>
     <t>CART-P04</t>
@@ -249,10 +300,13 @@
     <t>Quantity can be increased in cart</t>
   </si>
   <si>
-    <t>ADM-P07</t>
-  </si>
-  <si>
-    <t>Admin can delete a coupon</t>
+    <t>ADMIN — Products</t>
+  </si>
+  <si>
+    <t>ADM-P10</t>
+  </si>
+  <si>
+    <t>Products tab shows list of products</t>
   </si>
   <si>
     <t>CART-P05</t>
@@ -261,16 +315,28 @@
     <t>Item can be removed from cart</t>
   </si>
   <si>
+    <t>ADM-P11</t>
+  </si>
+  <si>
+    <t>Admin can create a new product</t>
+  </si>
+  <si>
     <t>CART-N02</t>
   </si>
   <si>
     <t>Empty cart shows empty state message</t>
   </si>
   <si>
-    <t>ADM-P08</t>
-  </si>
-  <si>
-    <t>Users tab shows list of registered users</t>
+    <t>CHECKOUT — Cart</t>
+  </si>
+  <si>
+    <t>CHK-P01</t>
+  </si>
+  <si>
+    <t>Checkout page loads for authenticated user with items in cart</t>
+  </si>
+  <si>
+    <t>CART — Promo</t>
   </si>
   <si>
     <t>CART-P06</t>
@@ -279,16 +345,25 @@
     <t>Valid coupon code applies discount to cart total</t>
   </si>
   <si>
+    <t>CHK-N01</t>
+  </si>
+  <si>
+    <t>Unauthenticated user is redirected from checkout</t>
+  </si>
+  <si>
+    <t>Error: [2mexpect([22m[31mpage[39m[2m).[22mtoHaveURL[2m([22m[32mexpected[39m[2m)[22m failed</t>
+  </si>
+  <si>
     <t>CART-N03</t>
   </si>
   <si>
     <t>Invalid coupon code shows error</t>
   </si>
   <si>
-    <t>ADM-P09</t>
-  </si>
-  <si>
-    <t>Users list shows at least one user (seed data)</t>
+    <t>CHK-N02</t>
+  </si>
+  <si>
+    <t>Proceeding to checkout with empty cart shows warning</t>
   </si>
   <si>
     <t>CART-P07</t>
@@ -297,67 +372,58 @@
     <t>Applied coupon can be removed</t>
   </si>
   <si>
-    <t>ADM-P10</t>
-  </si>
-  <si>
-    <t>Products tab shows list of products</t>
-  </si>
-  <si>
-    <t>CHK-P01</t>
-  </si>
-  <si>
-    <t>Checkout page loads for authenticated user with items in cart</t>
-  </si>
-  <si>
-    <t>ADM-P11</t>
-  </si>
-  <si>
-    <t>Admin can create a new product</t>
-  </si>
-  <si>
-    <t>CHK-N01</t>
-  </si>
-  <si>
-    <t>Unauthenticated user is redirected from checkout</t>
-  </si>
-  <si>
-    <t>CHK-N02</t>
-  </si>
-  <si>
-    <t>Proceeding to checkout with empty cart shows warning</t>
-  </si>
-  <si>
-    <t>Error: [2mexpect([22m[31mreceived[39m[2m).[22mtoBe[2m([22m[32mexpected[39m[2m) // Object.is equality[22m</t>
+    <t>CHECKOUT — Address</t>
+  </si>
+  <si>
+    <t>CHK-P02</t>
+  </si>
+  <si>
+    <t>User can select an existing address</t>
+  </si>
+  <si>
+    <t>has title</t>
   </si>
   <si>
     <t>—</t>
   </si>
   <si>
-    <t>has title</t>
-  </si>
-  <si>
     <t>get started link</t>
   </si>
   <si>
+    <t>PRODUCTS — Listing</t>
+  </si>
+  <si>
     <t>PROD-P01</t>
   </si>
   <si>
     <t>Products page loads and shows product cards</t>
   </si>
   <si>
+    <t>CHK-P03</t>
+  </si>
+  <si>
+    <t>User can add a new address during checkout</t>
+  </si>
+  <si>
     <t>PROD-P02</t>
   </si>
   <si>
     <t>Search returns filtered results</t>
   </si>
   <si>
-    <t>Error: locator.fill: Error: strict mode violation: getByPlaceholder(/search/i) resolved to 2 elements:</t>
-  </si>
-  <si>
-    <t>CHK-P02</t>
-  </si>
-  <si>
-    <t>User can select an existing address</t>
+    <t>CHK-N03</t>
+  </si>
+  <si>
+    <t>Cannot place order without selecting an address</t>
+  </si>
+  <si>
+    <t>CHECKOUT — Order</t>
+  </si>
+  <si>
+    <t>CHK-P04</t>
+  </si>
+  <si>
+    <t>Order confirmation page shows order details after successful (mocked) payment</t>
   </si>
   <si>
     <t>PROD-P03</t>
@@ -366,22 +432,22 @@
     <t>Category filter narrows products</t>
   </si>
   <si>
-    <t>CHK-P03</t>
-  </si>
-  <si>
-    <t>User can add a new address during checkout</t>
-  </si>
-  <si>
-    <t>CHK-N03</t>
-  </si>
-  <si>
-    <t>Cannot place order without selecting an address</t>
-  </si>
-  <si>
-    <t>CHK-P04</t>
-  </si>
-  <si>
-    <t>Order confirmation page shows order details after successful (mocked) payment</t>
+    <t>CHECKOUT — With</t>
+  </si>
+  <si>
+    <t>CHK-P05</t>
+  </si>
+  <si>
+    <t>Coupon discount is reflected in checkout summary</t>
+  </si>
+  <si>
+    <t>PROFILE — Auth</t>
+  </si>
+  <si>
+    <t>PROF-N01</t>
+  </si>
+  <si>
+    <t>Unauthenticated user is redirected to login</t>
   </si>
   <si>
     <t>PROD-N01</t>
@@ -390,16 +456,7 @@
     <t>Search with no results shows empty state</t>
   </si>
   <si>
-    <t>CHK-P05</t>
-  </si>
-  <si>
-    <t>Coupon discount is reflected in checkout summary</t>
-  </si>
-  <si>
-    <t>PROF-N01</t>
-  </si>
-  <si>
-    <t>Unauthenticated user is redirected to login</t>
+    <t>PROFILE — User</t>
   </si>
   <si>
     <t>PROF-P01</t>
@@ -408,6 +465,9 @@
     <t>Profile page shows user name and email</t>
   </si>
   <si>
+    <t>PRODUCTS — Detail</t>
+  </si>
+  <si>
     <t>PROD-P04</t>
   </si>
   <si>
@@ -420,22 +480,37 @@
     <t>Profile page shows My Account heading</t>
   </si>
   <si>
+    <t>PROD-P05</t>
+  </si>
+  <si>
+    <t>Product gallery image click changes main image</t>
+  </si>
+  <si>
+    <t>PROFILE — Order</t>
+  </si>
+  <si>
     <t>PROF-P03</t>
   </si>
   <si>
     <t>Orders tab shows order history</t>
   </si>
   <si>
+    <t>PROD-P06</t>
+  </si>
+  <si>
+    <t>Quantity selector can be incremented and decremented</t>
+  </si>
+  <si>
     <t>PROF-P04</t>
   </si>
   <si>
     <t>Order status stepper is visible on order cards</t>
   </si>
   <si>
-    <t>PROD-P05</t>
-  </si>
-  <si>
-    <t>Product gallery image click changes main image</t>
+    <t>PROD-N02</t>
+  </si>
+  <si>
+    <t>Navigating to non-existent product shows error state</t>
   </si>
   <si>
     <t>PROF-P05</t>
@@ -444,10 +519,16 @@
     <t>Cancelled orders show CANCELLED badge instead of stepper</t>
   </si>
   <si>
-    <t>PROD-P06</t>
-  </si>
-  <si>
-    <t>Quantity selector can be incremented and decremented</t>
+    <t>PRODUCTS — Variants</t>
+  </si>
+  <si>
+    <t>PROD-P07</t>
+  </si>
+  <si>
+    <t>Variant chips appear for products with variants</t>
+  </si>
+  <si>
+    <t>PROFILE — Addresses</t>
   </si>
   <si>
     <t>PROF-P06</t>
@@ -456,34 +537,37 @@
     <t>Addresses tab shows saved addresses</t>
   </si>
   <si>
+    <t>PROD-P08</t>
+  </si>
+  <si>
+    <t>Clicking color chip shows selected color</t>
+  </si>
+  <si>
+    <t>PROFILE — Wishlist</t>
+  </si>
+  <si>
     <t>PROF-P07</t>
   </si>
   <si>
     <t>Wishlist link is visible in sidebar</t>
   </si>
   <si>
+    <t>PRODUCTS — Reviews</t>
+  </si>
+  <si>
+    <t>PROD-P09</t>
+  </si>
+  <si>
+    <t>Reviews section is visible on product detail page</t>
+  </si>
+  <si>
     <t>PROF-P08</t>
   </si>
   <si>
     <t>Wishlist link navigates to /wishlist</t>
   </si>
   <si>
-    <t>PROD-N02</t>
-  </si>
-  <si>
-    <t>Navigating to non-existent product shows error state</t>
-  </si>
-  <si>
-    <t>PROD-P07</t>
-  </si>
-  <si>
-    <t>Variant chips appear for products with variants</t>
-  </si>
-  <si>
-    <t>PROD-P08</t>
-  </si>
-  <si>
-    <t>Clicking color chip shows selected color</t>
+    <t>PROFILE — Logout</t>
   </si>
   <si>
     <t>PROF-P09</t>
@@ -492,25 +576,31 @@
     <t>User can sign out from profile sidebar</t>
   </si>
   <si>
+    <t>PROD-P10</t>
+  </si>
+  <si>
+    <t>Unauthenticated user does NOT see write review form</t>
+  </si>
+  <si>
+    <t>WISHLIST — Auth</t>
+  </si>
+  <si>
     <t>WISH-N01</t>
   </si>
   <si>
+    <t>WISHLIST — Adding</t>
+  </si>
+  <si>
     <t>WISH-P01</t>
   </si>
   <si>
     <t>Logged-in user can add a product to wishlist via heart button</t>
   </si>
   <si>
-    <t>PROD-P09</t>
-  </si>
-  <si>
-    <t>Reviews section is visible on product detail page</t>
-  </si>
-  <si>
-    <t>PROD-P10</t>
-  </si>
-  <si>
-    <t>Unauthenticated user does NOT see write review form</t>
+    <t>PROD-P11</t>
+  </si>
+  <si>
+    <t>Logged-in user sees write review form</t>
   </si>
   <si>
     <t>WISH-P02</t>
@@ -519,36 +609,36 @@
     <t>Wishlist page shows saved products</t>
   </si>
   <si>
+    <t>PRODUCTS — Recommendations</t>
+  </si>
+  <si>
+    <t>PROD-P12</t>
+  </si>
+  <si>
+    <t>Recommendations carousel appears on product detail page when available</t>
+  </si>
+  <si>
     <t>WISH-P03</t>
   </si>
   <si>
     <t>Product can be removed from wishlist page</t>
   </si>
   <si>
-    <t>PROD-P11</t>
-  </si>
-  <si>
-    <t>Logged-in user sees write review form</t>
-  </si>
-  <si>
     <t>WISH-P04</t>
   </si>
   <si>
     <t>Add to Cart works from wishlist page</t>
   </si>
   <si>
-    <t>PROD-P12</t>
-  </si>
-  <si>
-    <t>Recommendations carousel appears on product detail page when available</t>
-  </si>
-  <si>
     <t>WISH-N02</t>
   </si>
   <si>
     <t>Empty wishlist shows empty state</t>
   </si>
   <si>
+    <t>WISHLIST — Toggle</t>
+  </si>
+  <si>
     <t>WISH-P05</t>
   </si>
   <si>
@@ -556,6 +646,15 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>66.7%</t>
+  </si>
+  <si>
+    <t>0.0%</t>
+  </si>
+  <si>
+    <t>100.0%</t>
   </si>
   <si>
     <t>TOTAL</t>
@@ -595,10 +694,10 @@
       <color rgb="FFFFFFFF"/>
     </font>
     <font>
-      <color rgb="FF1D4ED8"/>
+      <color rgb="FFB45309"/>
     </font>
     <font>
-      <color rgb="FFB45309"/>
+      <color rgb="FF1D4ED8"/>
     </font>
   </fonts>
   <fills count="7">
@@ -661,10 +760,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
@@ -1055,7 +1154,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="4">
-        <v>38</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1063,7 +1162,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="5">
-        <v>38</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1152,16 +1251,16 @@
         <v>24</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>8</v>
       </c>
       <c r="G2" s="7">
-        <v>5</v>
+        <v>3.3</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1169,103 +1268,103 @@
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>8</v>
       </c>
       <c r="G3">
-        <v>6.4</v>
+        <v>2.9</v>
       </c>
       <c r="H3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="G4" s="7">
-        <v>1.7</v>
+        <v>8.3</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>8</v>
       </c>
       <c r="G5">
-        <v>1.6</v>
+        <v>1.8</v>
       </c>
       <c r="H5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>28</v>
+        <v>37</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>8</v>
       </c>
       <c r="G6" s="7">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1273,74 +1372,74 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>24</v>
+        <v>39</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G7">
-        <v>6.8</v>
+        <v>9.2</v>
       </c>
       <c r="H7" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>24</v>
+        <v>43</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G8" s="7">
-        <v>9.5</v>
+        <v>6.6</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>24</v>
+        <v>46</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G9">
-        <v>7.1</v>
+        <v>9.7</v>
       </c>
       <c r="H9" t="s">
         <v>40</v>
@@ -1348,77 +1447,77 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="G10" s="7">
-        <v>1.5</v>
+        <v>6.6</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="G11">
-        <v>1.4</v>
+        <v>6.3</v>
       </c>
       <c r="H11" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>24</v>
+        <v>53</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G12" s="7">
-        <v>9.5</v>
+        <v>9.3</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>40</v>
@@ -1426,935 +1525,935 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="G13">
-        <v>1.6</v>
+        <v>6.7</v>
       </c>
       <c r="H13" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>28</v>
+        <v>58</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>8</v>
       </c>
       <c r="G14" s="7">
-        <v>2</v>
+        <v>1.2</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>28</v>
+        <v>60</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="E15" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="G15">
-        <v>2.5</v>
+        <v>9.4</v>
       </c>
       <c r="H15" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>9</v>
+        <v>25</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="G16" s="7">
-        <v>12.2</v>
+        <v>1.2</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D17" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>24</v>
       </c>
       <c r="E17" t="s">
-        <v>21</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>9</v>
+        <v>25</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="G17">
-        <v>12.3</v>
+        <v>2.1</v>
       </c>
       <c r="H17" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>24</v>
+        <v>67</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="G18" s="7">
-        <v>3.4</v>
+        <v>9.3</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="C19" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>24</v>
+        <v>70</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="E19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F19" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G19">
-        <v>11.5</v>
+        <v>11.4</v>
       </c>
       <c r="H19" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>24</v>
+        <v>73</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G20" s="7">
-        <v>11.4</v>
+        <v>9.7</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C21" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>24</v>
+        <v>76</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="E21" t="s">
-        <v>21</v>
-      </c>
-      <c r="F21" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G21">
-        <v>11.7</v>
+        <v>9.5</v>
       </c>
       <c r="H21" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>28</v>
+        <v>78</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F22" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G22" s="7">
-        <v>10.8</v>
+        <v>9.8</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="B23" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="C23" t="s">
-        <v>71</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>24</v>
+        <v>80</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="E23" t="s">
-        <v>21</v>
-      </c>
-      <c r="F23" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G23">
-        <v>11.7</v>
+        <v>9.9</v>
       </c>
       <c r="H23" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>24</v>
+        <v>82</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F24" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G24" s="7">
-        <v>11.4</v>
+        <v>9.1</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="B25" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="C25" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E25" t="s">
-        <v>21</v>
-      </c>
-      <c r="F25" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G25">
-        <v>11.4</v>
+        <v>10.8</v>
       </c>
       <c r="H25" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>21</v>
+        <v>85</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>24</v>
+        <v>87</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F26" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G26" s="7">
-        <v>11.5</v>
+        <v>9.2</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="B27" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="C27" t="s">
-        <v>79</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>24</v>
+        <v>90</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="E27" t="s">
-        <v>21</v>
-      </c>
-      <c r="F27" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G27">
-        <v>12.3</v>
+        <v>9.2</v>
       </c>
       <c r="H27" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>21</v>
+        <v>85</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>24</v>
+        <v>92</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F28" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G28" s="7">
-        <v>13.8</v>
+        <v>9.3</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="B29" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="C29" t="s">
-        <v>83</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>28</v>
+        <v>94</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="E29" t="s">
-        <v>21</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="G29">
-        <v>1.3</v>
+        <v>9</v>
       </c>
       <c r="H29" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>21</v>
+        <v>95</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>24</v>
+        <v>97</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F30" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G30" s="7">
-        <v>11.6</v>
+        <v>9.1</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="B31" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="C31" t="s">
-        <v>87</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>24</v>
+        <v>99</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="E31" t="s">
-        <v>21</v>
-      </c>
-      <c r="F31" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G31">
-        <v>11.3</v>
+        <v>9.3</v>
       </c>
       <c r="H31" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>21</v>
+        <v>95</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="G32" s="7">
-        <v>2.2</v>
+        <v>9.3</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="B33" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="C33" t="s">
-        <v>91</v>
-      </c>
-      <c r="D33" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="D33" s="10" t="s">
         <v>24</v>
       </c>
       <c r="E33" t="s">
-        <v>21</v>
-      </c>
-      <c r="F33" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G33">
-        <v>11.9</v>
+        <v>10</v>
       </c>
       <c r="H33" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>24</v>
+        <v>106</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F34" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G34" s="7">
-        <v>12.5</v>
+        <v>9.7</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>21</v>
+        <v>107</v>
       </c>
       <c r="B35" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="C35" t="s">
-        <v>95</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>24</v>
+        <v>109</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="E35" t="s">
-        <v>21</v>
-      </c>
-      <c r="F35" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F35" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G35">
-        <v>12.8</v>
+        <v>9.6</v>
       </c>
       <c r="H35" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="D36" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F36" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F36" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G36" s="7">
-        <v>14.6</v>
+        <v>6.2</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>57</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>21</v>
+        <v>107</v>
       </c>
       <c r="B37" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="C37" t="s">
-        <v>99</v>
-      </c>
-      <c r="D37" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D37" s="10" t="s">
         <v>24</v>
       </c>
       <c r="E37" t="s">
-        <v>21</v>
-      </c>
-      <c r="F37" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F37" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G37">
-        <v>12.5</v>
+        <v>9.9</v>
       </c>
       <c r="H37" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>28</v>
+        <v>116</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F38" s="9" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="G38" s="7">
-        <v>3.4</v>
+        <v>9.8</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>21</v>
+        <v>107</v>
       </c>
       <c r="B39" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="C39" t="s">
-        <v>103</v>
-      </c>
-      <c r="D39" s="10" t="s">
-        <v>28</v>
+        <v>118</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="E39" t="s">
-        <v>21</v>
-      </c>
-      <c r="F39" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F39" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G39">
-        <v>2.6</v>
+        <v>9.7</v>
       </c>
       <c r="H39" t="s">
-        <v>104</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>21</v>
+        <v>119</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>24</v>
+        <v>121</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F40" s="9" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="G40" s="7">
-        <v>1.2</v>
+        <v>10</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>21</v>
+        <v>122</v>
       </c>
       <c r="B41" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="C41" t="s">
-        <v>107</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>24</v>
+        <v>122</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="E41" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F41" s="9" t="s">
         <v>8</v>
       </c>
       <c r="G41">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="H41" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>21</v>
+        <v>124</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>24</v>
+        <v>124</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F42" s="9" t="s">
         <v>8</v>
       </c>
       <c r="G42" s="7">
-        <v>1.9</v>
+        <v>1.5</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>21</v>
+        <v>125</v>
       </c>
       <c r="B43" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="C43" t="s">
-        <v>111</v>
-      </c>
-      <c r="D43" s="12" t="s">
-        <v>24</v>
+        <v>127</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="E43" t="s">
-        <v>21</v>
-      </c>
-      <c r="F43" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F43" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G43">
-        <v>1.6</v>
+        <v>10</v>
       </c>
       <c r="H43" t="s">
-        <v>112</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>21</v>
+        <v>119</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>24</v>
+        <v>129</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F44" s="9" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="F44" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="G44" s="7">
-        <v>4.5</v>
+        <v>10.4</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>21</v>
+        <v>125</v>
       </c>
       <c r="B45" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="C45" t="s">
-        <v>116</v>
-      </c>
-      <c r="D45" s="12" t="s">
-        <v>24</v>
+        <v>131</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="E45" t="s">
-        <v>21</v>
-      </c>
-      <c r="F45" s="9" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="F45" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="G45">
-        <v>2</v>
+        <v>10.7</v>
       </c>
       <c r="H45" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>21</v>
+        <v>119</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>118</v>
+        <v>133</v>
       </c>
       <c r="D46" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F46" s="9" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="F46" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="G46" s="7">
-        <v>4.3</v>
+        <v>9.8</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>21</v>
+        <v>134</v>
       </c>
       <c r="B47" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="C47" t="s">
-        <v>120</v>
-      </c>
-      <c r="D47" s="10" t="s">
-        <v>28</v>
+        <v>136</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="E47" t="s">
-        <v>21</v>
-      </c>
-      <c r="F47" s="9" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="F47" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="G47">
-        <v>3.7</v>
+        <v>1.7</v>
       </c>
       <c r="H47" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>21</v>
+        <v>125</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>24</v>
+        <v>138</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F48" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F48" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G48" s="7">
-        <v>1.9</v>
+        <v>8</v>
       </c>
       <c r="H48" s="7" t="s">
         <v>40</v>
@@ -2362,25 +2461,25 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>21</v>
+        <v>139</v>
       </c>
       <c r="B49" t="s">
-        <v>123</v>
+        <v>140</v>
       </c>
       <c r="C49" t="s">
-        <v>124</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>28</v>
+        <v>141</v>
+      </c>
+      <c r="D49" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="E49" t="s">
-        <v>21</v>
-      </c>
-      <c r="F49" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F49" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G49">
-        <v>9.3</v>
+        <v>9.6</v>
       </c>
       <c r="H49" t="s">
         <v>40</v>
@@ -2388,77 +2487,77 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>21</v>
+        <v>142</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="D50" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F50" s="9" t="s">
         <v>8</v>
       </c>
       <c r="G50" s="7">
-        <v>4.7</v>
+        <v>1.6</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>21</v>
+        <v>125</v>
       </c>
       <c r="B51" t="s">
-        <v>127</v>
+        <v>145</v>
       </c>
       <c r="C51" t="s">
-        <v>128</v>
+        <v>146</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E51" t="s">
-        <v>21</v>
-      </c>
-      <c r="F51" s="9" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="F51" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="G51">
-        <v>1.7</v>
+        <v>9.5</v>
       </c>
       <c r="H51" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>21</v>
+        <v>147</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>129</v>
+        <v>148</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>24</v>
+        <v>149</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F52" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F52" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G52" s="7">
-        <v>2</v>
+        <v>9.5</v>
       </c>
       <c r="H52" s="7" t="s">
         <v>40</v>
@@ -2466,181 +2565,181 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>21</v>
+        <v>150</v>
       </c>
       <c r="B53" t="s">
-        <v>131</v>
+        <v>151</v>
       </c>
       <c r="C53" t="s">
-        <v>132</v>
-      </c>
-      <c r="D53" s="12" t="s">
-        <v>24</v>
+        <v>152</v>
+      </c>
+      <c r="D53" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="E53" t="s">
-        <v>21</v>
-      </c>
-      <c r="F53" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F53" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G53">
-        <v>7.2</v>
+        <v>11.1</v>
       </c>
       <c r="H53" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>21</v>
+        <v>147</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>133</v>
+        <v>153</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>24</v>
+        <v>154</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F54" s="9" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="F54" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="G54" s="7">
-        <v>1.9</v>
+        <v>9.7</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>21</v>
+        <v>150</v>
       </c>
       <c r="B55" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="C55" t="s">
-        <v>136</v>
-      </c>
-      <c r="D55" s="12" t="s">
-        <v>24</v>
+        <v>156</v>
+      </c>
+      <c r="D55" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="E55" t="s">
-        <v>21</v>
-      </c>
-      <c r="F55" s="9" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="F55" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="G55">
-        <v>3.3</v>
+        <v>11.1</v>
       </c>
       <c r="H55" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>21</v>
+        <v>157</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>137</v>
+        <v>158</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="D56" s="8" t="s">
-        <v>24</v>
+        <v>159</v>
+      </c>
+      <c r="D56" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F56" s="9" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="F56" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="G56" s="7">
-        <v>2</v>
+        <v>9.6</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>21</v>
+        <v>150</v>
       </c>
       <c r="B57" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="C57" t="s">
-        <v>140</v>
-      </c>
-      <c r="D57" s="12" t="s">
-        <v>24</v>
+        <v>161</v>
+      </c>
+      <c r="D57" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="E57" t="s">
-        <v>21</v>
-      </c>
-      <c r="F57" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F57" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G57">
-        <v>6.6</v>
+        <v>11.1</v>
       </c>
       <c r="H57" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>21</v>
+        <v>157</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="D58" s="8" t="s">
-        <v>24</v>
+        <v>163</v>
+      </c>
+      <c r="D58" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F58" s="9" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="F58" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="G58" s="7">
-        <v>2.1</v>
+        <v>9.7</v>
       </c>
       <c r="H58" s="7" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>21</v>
+        <v>150</v>
       </c>
       <c r="B59" t="s">
-        <v>143</v>
+        <v>164</v>
       </c>
       <c r="C59" t="s">
-        <v>144</v>
-      </c>
-      <c r="D59" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="D59" s="10" t="s">
         <v>24</v>
       </c>
       <c r="E59" t="s">
-        <v>21</v>
-      </c>
-      <c r="F59" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F59" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G59">
-        <v>7.4</v>
+        <v>9.2</v>
       </c>
       <c r="H59" t="s">
         <v>40</v>
@@ -2648,181 +2747,181 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>21</v>
+        <v>157</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="D60" s="8" t="s">
-        <v>24</v>
+        <v>167</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F60" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F60" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G60" s="7">
-        <v>11.8</v>
+        <v>9.6</v>
       </c>
       <c r="H60" s="7" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>21</v>
+        <v>168</v>
       </c>
       <c r="B61" t="s">
-        <v>147</v>
+        <v>169</v>
       </c>
       <c r="C61" t="s">
-        <v>148</v>
-      </c>
-      <c r="D61" s="12" t="s">
-        <v>24</v>
+        <v>170</v>
+      </c>
+      <c r="D61" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="E61" t="s">
-        <v>21</v>
-      </c>
-      <c r="F61" s="9" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="F61" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="G61">
-        <v>2.1</v>
+        <v>11.2</v>
       </c>
       <c r="H61" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>21</v>
+        <v>171</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>149</v>
+        <v>172</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="D62" s="8" t="s">
-        <v>24</v>
+        <v>173</v>
+      </c>
+      <c r="D62" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F62" s="9" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="F62" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="G62" s="7">
-        <v>2.8</v>
+        <v>9.8</v>
       </c>
       <c r="H62" s="7" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>21</v>
+        <v>168</v>
       </c>
       <c r="B63" t="s">
-        <v>151</v>
+        <v>174</v>
       </c>
       <c r="C63" t="s">
-        <v>152</v>
-      </c>
-      <c r="D63" s="10" t="s">
-        <v>28</v>
+        <v>175</v>
+      </c>
+      <c r="D63" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="E63" t="s">
-        <v>21</v>
-      </c>
-      <c r="F63" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F63" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G63">
-        <v>9.1</v>
+        <v>11.4</v>
       </c>
       <c r="H63" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>21</v>
+        <v>176</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>153</v>
+        <v>177</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="D64" s="8" t="s">
-        <v>24</v>
+        <v>178</v>
+      </c>
+      <c r="D64" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F64" s="9" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="F64" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="G64" s="7">
-        <v>1.9</v>
+        <v>9.7</v>
       </c>
       <c r="H64" s="7" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>21</v>
+        <v>179</v>
       </c>
       <c r="B65" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
       <c r="C65" t="s">
-        <v>156</v>
-      </c>
-      <c r="D65" s="12" t="s">
-        <v>24</v>
+        <v>181</v>
+      </c>
+      <c r="D65" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="E65" t="s">
-        <v>21</v>
-      </c>
-      <c r="F65" s="9" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="F65" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="G65">
-        <v>1.2</v>
+        <v>11.3</v>
       </c>
       <c r="H65" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>21</v>
+        <v>176</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>157</v>
+        <v>182</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="D66" s="8" t="s">
-        <v>24</v>
+        <v>183</v>
+      </c>
+      <c r="D66" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F66" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F66" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G66" s="7">
-        <v>8.4</v>
+        <v>10.1</v>
       </c>
       <c r="H66" s="7" t="s">
         <v>40</v>
@@ -2830,259 +2929,259 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>21</v>
+        <v>184</v>
       </c>
       <c r="B67" t="s">
-        <v>159</v>
+        <v>185</v>
       </c>
       <c r="C67" t="s">
-        <v>52</v>
-      </c>
-      <c r="D67" s="10" t="s">
-        <v>28</v>
+        <v>186</v>
+      </c>
+      <c r="D67" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="E67" t="s">
-        <v>21</v>
-      </c>
-      <c r="F67" s="9" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="F67" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="G67">
-        <v>1.8</v>
+        <v>9.6</v>
       </c>
       <c r="H67" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>21</v>
+        <v>179</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>160</v>
+        <v>187</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="D68" s="8" t="s">
-        <v>24</v>
+        <v>188</v>
+      </c>
+      <c r="D68" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F68" s="9" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="F68" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="G68" s="7">
-        <v>2.2</v>
+        <v>11.4</v>
       </c>
       <c r="H68" s="7" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>21</v>
+        <v>189</v>
       </c>
       <c r="B69" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="C69" t="s">
-        <v>163</v>
-      </c>
-      <c r="D69" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D69" s="10" t="s">
         <v>24</v>
       </c>
       <c r="E69" t="s">
-        <v>21</v>
-      </c>
-      <c r="F69" s="13" t="s">
-        <v>9</v>
+        <v>25</v>
+      </c>
+      <c r="F69" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="G69">
-        <v>9.1</v>
+        <v>2.3</v>
       </c>
       <c r="H69" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>21</v>
+        <v>191</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>164</v>
+        <v>192</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="D70" s="8" t="s">
-        <v>24</v>
+        <v>193</v>
+      </c>
+      <c r="D70" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F70" s="9" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="F70" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="G70" s="7">
-        <v>1.5</v>
+        <v>10.1</v>
       </c>
       <c r="H70" s="7" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>21</v>
+        <v>179</v>
       </c>
       <c r="B71" t="s">
-        <v>166</v>
+        <v>194</v>
       </c>
       <c r="C71" t="s">
-        <v>167</v>
-      </c>
-      <c r="D71" s="12" t="s">
-        <v>24</v>
+        <v>195</v>
+      </c>
+      <c r="D71" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="E71" t="s">
-        <v>21</v>
-      </c>
-      <c r="F71" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F71" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G71">
-        <v>8.6</v>
+        <v>13.9</v>
       </c>
       <c r="H71" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>21</v>
+        <v>191</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>168</v>
+        <v>196</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="D72" s="8" t="s">
-        <v>24</v>
+        <v>197</v>
+      </c>
+      <c r="D72" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F72" s="9" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="F72" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="G72" s="7">
-        <v>3.2</v>
+        <v>9.7</v>
       </c>
       <c r="H72" s="7" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>21</v>
+        <v>198</v>
       </c>
       <c r="B73" t="s">
-        <v>170</v>
+        <v>199</v>
       </c>
       <c r="C73" t="s">
-        <v>171</v>
-      </c>
-      <c r="D73" s="12" t="s">
-        <v>24</v>
+        <v>200</v>
+      </c>
+      <c r="D73" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="E73" t="s">
-        <v>21</v>
-      </c>
-      <c r="F73" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F73" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G73">
-        <v>10.6</v>
+        <v>11.4</v>
       </c>
       <c r="H73" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
-        <v>21</v>
+        <v>191</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>172</v>
+        <v>201</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="D74" s="8" t="s">
-        <v>24</v>
+        <v>202</v>
+      </c>
+      <c r="D74" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F74" s="9" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="F74" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="G74" s="7">
-        <v>3.8</v>
+        <v>9.9</v>
       </c>
       <c r="H74" s="7" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>21</v>
+        <v>191</v>
       </c>
       <c r="B75" t="s">
-        <v>174</v>
+        <v>203</v>
       </c>
       <c r="C75" t="s">
-        <v>175</v>
-      </c>
-      <c r="D75" s="12" t="s">
-        <v>24</v>
+        <v>204</v>
+      </c>
+      <c r="D75" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="E75" t="s">
-        <v>21</v>
-      </c>
-      <c r="F75" s="9" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="F75" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="G75">
-        <v>3.8</v>
+        <v>9.7</v>
       </c>
       <c r="H75" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
-        <v>21</v>
+        <v>191</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>176</v>
+        <v>205</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="D76" s="11" t="s">
-        <v>28</v>
+        <v>206</v>
+      </c>
+      <c r="D76" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="E76" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F76" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F76" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G76" s="7">
-        <v>9</v>
+        <v>9.6</v>
       </c>
       <c r="H76" s="7" t="s">
         <v>40</v>
@@ -3090,28 +3189,28 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>21</v>
+        <v>207</v>
       </c>
       <c r="B77" t="s">
-        <v>178</v>
+        <v>208</v>
       </c>
       <c r="C77" t="s">
-        <v>179</v>
-      </c>
-      <c r="D77" s="12" t="s">
-        <v>24</v>
+        <v>209</v>
+      </c>
+      <c r="D77" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="E77" t="s">
-        <v>21</v>
-      </c>
-      <c r="F77" s="9" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="F77" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="G77">
-        <v>2.2</v>
+        <v>9.7</v>
       </c>
       <c r="H77" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -3123,7 +3222,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F35"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
@@ -3136,7 +3235,7 @@
         <v>13</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>180</v>
+        <v>210</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>8</v>
@@ -3156,38 +3255,678 @@
         <v>21</v>
       </c>
       <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13" s="5">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14" s="5">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15" s="5">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16" s="5">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>122</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>125</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" s="5">
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>134</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20" s="5">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>139</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" s="5">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>142</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>147</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23" s="5">
+        <v>2</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>150</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24" s="5">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>157</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25" s="5">
+        <v>3</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>168</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26" s="5">
+        <v>2</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>171</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27" s="5">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>176</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28" s="5">
+        <v>2</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>179</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29" s="5">
+        <v>3</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>184</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30" s="5">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>189</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>191</v>
+      </c>
+      <c r="B32">
+        <v>5</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32" s="5">
+        <v>5</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>198</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33" s="5">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>207</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34" s="5">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="B35" s="15">
         <v>76</v>
       </c>
-      <c r="C2">
-        <v>38</v>
-      </c>
-      <c r="D2" s="5">
-        <v>38</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="B3" s="15">
-        <v>76</v>
-      </c>
-      <c r="C3" s="15">
-        <v>38</v>
-      </c>
-      <c r="D3" s="15">
-        <v>38</v>
-      </c>
-      <c r="E3" s="15">
-        <v>0</v>
-      </c>
-      <c r="F3" s="15" t="s">
+      <c r="C35" s="15">
+        <v>11</v>
+      </c>
+      <c r="D35" s="15">
+        <v>65</v>
+      </c>
+      <c r="E35" s="15">
+        <v>0</v>
+      </c>
+      <c r="F35" s="15" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: implement AI Shopping Assistant and comprehensive API test suite
</commit_message>
<xml_diff>
--- a/frontend/tests/test-results/ShopEase_TestReport.xlsx
+++ b/frontend/tests/test-results/ShopEase_TestReport.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="39">
   <si>
     <t>ShopEase E2E Test Execution Report</t>
   </si>
@@ -21,13 +21,13 @@
     <t>Generated:</t>
   </si>
   <si>
-    <t>24/2/2026, 10:25:08 pm</t>
+    <t>25/2/2026, 9:20:04 am</t>
   </si>
   <si>
     <t>Duration:</t>
   </si>
   <si>
-    <t>75s</t>
+    <t>19s</t>
   </si>
   <si>
     <t>Metric</t>
@@ -51,7 +51,7 @@
     <t>Pass Rate</t>
   </si>
   <si>
-    <t>16.7%</t>
+    <t>25.0%</t>
   </si>
   <si>
     <t>Module</t>
@@ -78,13 +78,13 @@
     <t>Error</t>
   </si>
   <si>
-    <t>M</t>
+    <t>S</t>
   </si>
   <si>
     <t>—</t>
   </si>
   <si>
-    <t>AI-N01: Chat bubble hidden when not logged in</t>
+    <t>Login with valid credentials</t>
   </si>
   <si>
     <t>Positive</t>
@@ -93,25 +93,37 @@
     <t>chromium</t>
   </si>
   <si>
+    <t>Error: [2mexpect([22m[31mreceived[39m[2m).[22mtoBeDefined[2m()[22m</t>
+  </si>
+  <si>
+    <t>Login with invalid password</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>AI-P01: Chat bubble visible after login</t>
-  </si>
-  <si>
-    <t>TimeoutError: page.fill: Timeout 10000ms exceeded.</t>
-  </si>
-  <si>
-    <t>AI-P02: Click bubble opens chat panel</t>
-  </si>
-  <si>
-    <t>AI-N02: Empty message cannot be sent</t>
-  </si>
-  <si>
-    <t>AI-P03: Send message gets AI response</t>
-  </si>
-  <si>
-    <t>AI-P04: Close and reopen preserves chat</t>
+    <t>Get profile with valid token</t>
+  </si>
+  <si>
+    <t>Get profile without token</t>
+  </si>
+  <si>
+    <t>Error: [2mexpect([22m[31mreceived[39m[2m).[22mtoBe[2m([22m[32mexpected[39m[2m) // Object.is equality[22m</t>
+  </si>
+  <si>
+    <t>Get all paginated products</t>
+  </si>
+  <si>
+    <t>SyntaxError: Unexpected non-whitespace character after JSON at position 165930 (line 1 column 165931)</t>
+  </si>
+  <si>
+    <t>Get non-existent product</t>
+  </si>
+  <si>
+    <t>Chat setup missing message body</t>
+  </si>
+  <si>
+    <t>Get AI conversations</t>
   </si>
   <si>
     <t>Total</t>
@@ -124,7 +136,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -156,8 +168,11 @@
     <font>
       <color rgb="FF1D4ED8"/>
     </font>
+    <font>
+      <color rgb="FF92400E"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,12 +191,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFEE2E2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFD1FAE5"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFEE2E2"/>
+        <fgColor rgb="FFFEF3C7"/>
       </patternFill>
     </fill>
     <fill>
@@ -202,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -216,11 +236,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -601,7 +622,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -609,7 +630,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -617,7 +638,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -625,7 +646,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -647,7 +668,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -709,10 +730,10 @@
         <v>25</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G2" s="7">
-        <v>7.4</v>
+        <v>0.3</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>26</v>
@@ -735,10 +756,10 @@
         <v>25</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G3">
-        <v>11.5</v>
+        <v>0.3</v>
       </c>
       <c r="H3" t="s">
         <v>28</v>
@@ -760,11 +781,11 @@
       <c r="E4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>9</v>
+      <c r="F4" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="G4" s="7">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>28</v>
@@ -786,14 +807,14 @@
       <c r="E5" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="9" t="s">
         <v>9</v>
       </c>
       <c r="G5">
-        <v>11</v>
+        <v>0.1</v>
       </c>
       <c r="H5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -804,7 +825,7 @@
         <v>22</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>24</v>
@@ -812,14 +833,14 @@
       <c r="E6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="9" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="7">
-        <v>11.2</v>
+        <v>0.3</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -830,7 +851,7 @@
         <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>24</v>
@@ -839,12 +860,64 @@
         <v>25</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G7">
-        <v>11</v>
+        <v>0.1</v>
       </c>
       <c r="H7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="7">
+        <v>0</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
         <v>28</v>
       </c>
     </row>
@@ -865,23 +938,23 @@
     <col min="6" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="12" t="s">
+      <c r="B1" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="13" t="s">
         <v>11</v>
       </c>
     </row>
@@ -890,38 +963,38 @@
         <v>21</v>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="13">
-        <v>6</v>
-      </c>
-      <c r="C3" s="13">
-        <v>1</v>
-      </c>
-      <c r="D3" s="13">
-        <v>5</v>
-      </c>
-      <c r="E3" s="13">
-        <v>0</v>
-      </c>
-      <c r="F3" s="13" t="s">
+    <row r="3" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="14">
+        <v>8</v>
+      </c>
+      <c r="C3" s="14">
+        <v>2</v>
+      </c>
+      <c r="D3" s="14">
+        <v>3</v>
+      </c>
+      <c r="E3" s="14">
+        <v>3</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>